<commit_message>
Modificacion del excel y del programa js
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,25 +1,217 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiubaar-my.sharepoint.com/personal/jquijano_fi_uba_ar/Documents/Curso Front End -Ticmas Academy/Proyecto CV/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A823186-F505-4059-9B9C-366679C6EA53}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiencia" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Juan Pablo Quijano Cuman</t>
+  </si>
+  <si>
+    <t>Profesión</t>
+  </si>
+  <si>
+    <t>Estudiante de Ingeniería mecánica</t>
+  </si>
+  <si>
+    <t>Período</t>
+  </si>
+  <si>
+    <t>Lugar</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Nacionalidad</t>
+  </si>
+  <si>
+    <t>Documento</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Estado_civil</t>
+  </si>
+  <si>
+    <t>Fecha_Nacimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresar al mercado laboral con el fin de aprender y adquirir experiencia relacionada a la ingeniería mecánica. </t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Domicilio</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>Alberti  134,  Piso  7° “B”– CAPITAL FEDERAL</t>
+  </si>
+  <si>
+    <t>juanpquijano@outlook.com</t>
+  </si>
+  <si>
+    <t>11-6160-3797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 - actualidad  </t>
+  </si>
+  <si>
+    <t>Me encuentro cursando el 4to año de la carrera.</t>
+  </si>
+  <si>
+    <t>Educacion</t>
+  </si>
+  <si>
+    <t>Facultad de Ingeniería - UBA</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Colegio San José de Buenos Aires</t>
+  </si>
+  <si>
+    <t>2013-2017</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>Ingeniería Mecánica</t>
+  </si>
+  <si>
+    <t>Secundario completo</t>
+  </si>
+  <si>
+    <t>Bachiller con orientación en Ciencias Exactas aplicadas a técnicas administrativo-contables. Promedio: 9,31 - Diploma de Honor</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>Ingles</t>
+  </si>
+  <si>
+    <t>Nivel B2</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Nativo</t>
+  </si>
+  <si>
+    <t>Estudio Contable Lesta, Calello, De Chiara</t>
+  </si>
+  <si>
+    <t>2018 - 2021</t>
+  </si>
+  <si>
+    <t>Administrativo</t>
+  </si>
+  <si>
+    <t>Realizaba tareas de análisis y confección de informes de Concursos Preventivos y Quiebras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repartidor </t>
+  </si>
+  <si>
+    <t>Wait For It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tareas de reparto de alimentos por la zona de microcentro. </t>
+  </si>
+  <si>
+    <t>Capacitacion</t>
+  </si>
+  <si>
+    <t>Manejo de AutoCAD Mechanical (UBA)</t>
+  </si>
+  <si>
+    <t>Curso Data Science and Machine Learning in Python</t>
+  </si>
+  <si>
+    <t>Curso Automación y Control: Módulo PLC (UTN)</t>
+  </si>
+  <si>
+    <t>Excelente manejo de Paquete de Office</t>
+  </si>
+  <si>
+    <t>Excel, Word, PowerPoint</t>
+  </si>
+  <si>
+    <t>Introducción a la programación de PLC. Diagramas lógicos, esquemas de conexión, lenguaje Ladder, Contadores, Timers, Internal Relays.</t>
+  </si>
+  <si>
+    <t>Dictado en inglés por la Fachhochschule Dortmund - Alemania. Manejo  de  librerías  Numpy,  Pandas, 
+Matplotlib y Scikit.learn.</t>
+  </si>
+  <si>
+    <t>Ingresar al mercado laboral con el fin de aprender y adquirir experiencia relacionada a la ingeniería mecánica.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,17 +237,518 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="26">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +759,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A13:K14" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="24">
+  <autoFilter ref="A13:K14" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesión" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="email" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A1:F11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:F11" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="5">
+      <calculatedColumnFormula>+B1+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Período" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripción" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +1060,410 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42176358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>36486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="9">
+        <v>42176358</v>
+      </c>
+      <c r="E14" s="9">
+        <v>23</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="11">
+        <v>36486</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D90C00-5FCB-4F90-B5F9-62EA9D964F59}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1">
+        <f>+B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1">
+        <f>+B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <f>+B6+1</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1">
+        <f>+B8+1</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ref="B10:B11" si="0">+B9+1</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
JS: Se agregó una función para crear tarjetas autocompletadas y una función para autocompletar la información personal. Excel: Se completó con los datos personales y de experiencia para poder extraer la información en formato JSON con un script propio de excel. HTML: Se quitaron las tarjetas para que se completen directamente con el código cuando se abre la página.
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiubaar-my.sharepoint.com/personal/jquijano_fi_uba_ar/Documents/Curso Front End -Ticmas Academy/Proyecto CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A823186-F505-4059-9B9C-366679C6EA53}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE3CD8FE-1999-40B9-84BB-547EA0C86218}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Experiencia" sheetId="2" r:id="rId2"/>
+    <sheet name="Info_personal" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,19 +45,10 @@
     <t>Juan Pablo Quijano Cuman</t>
   </si>
   <si>
-    <t>Profesión</t>
-  </si>
-  <si>
     <t>Estudiante de Ingeniería mecánica</t>
   </si>
   <si>
-    <t>Período</t>
-  </si>
-  <si>
     <t>Lugar</t>
-  </si>
-  <si>
-    <t>Descripción</t>
   </si>
   <si>
     <t>Trabajo</t>
@@ -206,6 +197,15 @@
   </si>
   <si>
     <t>Ingresar al mercado laboral con el fin de aprender y adquirir experiencia relacionada a la ingeniería mecánica.</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Profesion</t>
   </si>
 </sst>
 </file>
@@ -352,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -365,12 +365,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="25">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -392,106 +525,191 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -502,22 +720,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -527,225 +729,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -762,37 +745,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A13:K14" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A13:K14" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A13:K14" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesión" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="email" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="email" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A1:F11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A1:F11" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F11" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="4">
       <calculatedColumnFormula>+B1+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Período" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripción" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Periodo" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripcion" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1063,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,23 +1068,23 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>42176358</v>
@@ -1109,7 +1092,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>23</v>
@@ -1117,15 +1100,15 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>36486</v>
@@ -1133,34 +1116,34 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1168,34 +1151,34 @@
         <v>0</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1203,10 +1186,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" s="9">
         <v>42176358</v>
@@ -1215,22 +1198,22 @@
         <v>23</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G14" s="11">
         <v>36486</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1245,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D90C00-5FCB-4F90-B5F9-62EA9D964F59}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,68 +1241,68 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <f>+B2+1</f>
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>34</v>
+      <c r="F3" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1327,15 +1310,15 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>+B4+1</f>
@@ -1344,35 +1327,35 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <f>+B6+1</f>
@@ -1382,18 +1365,18 @@
         <v>2018</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1401,13 +1384,13 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1">
         <f>+B8+1</f>
@@ -1418,15 +1401,15 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ref="B10:B11" si="0">+B9+1</f>
@@ -1437,15 +1420,15 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="9">
         <f t="shared" si="0"/>
@@ -1454,10 +1437,10 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se realizaron varios cambios: 1) Se agregó una foto de la paleta de colores utilizada en la carpeta 'imagenes'. 2) Se agregaron iconos con información personal (telefono, Dirección, mail). 3) Se cambió el estilo de la página agregando clases a estilos.css.4) Se agregó el botón 'Contáctame' pero sin funcionalidad.
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiubaar-my.sharepoint.com/personal/jquijano_fi_uba_ar/Documents/Curso Front End -Ticmas Academy/Proyecto CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE3CD8FE-1999-40B9-84BB-547EA0C86218}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B303525-28A3-4F4D-814B-ED1FCD948CD7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info_personal" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Nombre</t>
   </si>
@@ -206,14 +206,25 @@
   </si>
   <si>
     <t>Profesion</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -352,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -365,6 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1136,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -1216,10 +1228,14 @@
         <v>52</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1228,13 +1244,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D90C00-5FCB-4F90-B5F9-62EA9D964F59}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
     <col min="5" max="5" width="43.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Se completó la información del archivo de excel y del archivo de texto. Se lo movió el archivo txt a la carpeta principal
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiubaar-my.sharepoint.com/personal/jquijano_fi_uba_ar/Documents/Curso Front End -Ticmas Academy/Proyecto CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B303525-28A3-4F4D-814B-ED1FCD948CD7}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15712030-EB17-41A1-A4EF-8D2FC204D5F6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Info_personal" sheetId="1" r:id="rId1"/>
+    <sheet name="info_personal" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Capacidades" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>Nombre</t>
   </si>
@@ -93,18 +94,12 @@
     <t>Celular</t>
   </si>
   <si>
-    <t>Alberti  134,  Piso  7° “B”– CAPITAL FEDERAL</t>
-  </si>
-  <si>
     <t>juanpquijano@outlook.com</t>
   </si>
   <si>
     <t>11-6160-3797</t>
   </si>
   <si>
-    <t xml:space="preserve">2018 - actualidad  </t>
-  </si>
-  <si>
     <t>Me encuentro cursando el 4to año de la carrera.</t>
   </si>
   <si>
@@ -120,9 +115,6 @@
     <t>Colegio San José de Buenos Aires</t>
   </si>
   <si>
-    <t>2013-2017</t>
-  </si>
-  <si>
     <t>Titulo</t>
   </si>
   <si>
@@ -153,13 +145,7 @@
     <t>Estudio Contable Lesta, Calello, De Chiara</t>
   </si>
   <si>
-    <t>2018 - 2021</t>
-  </si>
-  <si>
     <t>Administrativo</t>
-  </si>
-  <si>
-    <t>Realizaba tareas de análisis y confección de informes de Concursos Preventivos y Quiebras.</t>
   </si>
   <si>
     <t xml:space="preserve">Repartidor </t>
@@ -209,13 +195,100 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
+    <t>/juan-pablo-quijano-cuman</t>
+  </si>
+  <si>
+    <t>Capacidades</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Proactivo</t>
+  </si>
+  <si>
+    <t>Trabajo en equipo</t>
+  </si>
+  <si>
+    <t>Autodidacta</t>
+  </si>
+  <si>
+    <t>Capacidad de análisis</t>
+  </si>
+  <si>
+    <t>Organizado</t>
+  </si>
+  <si>
+    <t>Resolución de problemas</t>
+  </si>
+  <si>
+    <t>Alberti  134,  Piso  7° “B”– CABA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marzo 2018 - actualidad  </t>
+  </si>
+  <si>
+    <t>Febrero 2013 - Diciembre 2017</t>
+  </si>
+  <si>
+    <t>Mayo 2018 - Julio 2021</t>
+  </si>
+  <si>
+    <t>Febrero - Julio 2022</t>
+  </si>
+  <si>
+    <t>Enero - Julio 2018</t>
+  </si>
+  <si>
+    <t>Septiembre - Noviembre 2022</t>
+  </si>
+  <si>
+    <t>Diseño de piezas mecánicas en vista plana, manejo de layers, acotación según normas</t>
+  </si>
+  <si>
+    <t>Tareas de análisis y confección de informes de Concursos Preventivos y Quiebras. Análisis en Excel de la documentación respaldatoria del crédito con funciones matemáticas. Informe en Word detallando el porqué de la rechazo o verificación parcial o total del crédito.</t>
+  </si>
+  <si>
+    <t>Enero 2023 - actualidad</t>
+  </si>
+  <si>
+    <t>Tetra Pak SRL</t>
+  </si>
+  <si>
+    <t>Pasante de Automation</t>
+  </si>
+  <si>
+    <t>Confección de pantallas Intouch para control de máquinas. Proceso desde P&amp;ID en AutoCAD hasta pantalla funcional acoplada a la máquina.</t>
+  </si>
+  <si>
+    <t>Info_personal</t>
+  </si>
+  <si>
+    <t>Experiencia</t>
+  </si>
+  <si>
+    <t>Diciembre 2022 - Enero 2023</t>
+  </si>
+  <si>
+    <t>Ticmas Academy</t>
+  </si>
+  <si>
+    <t>Curso Primeros pasos del desarrollo FrontEnd</t>
+  </si>
+  <si>
+    <t>Programa "Argentina Programa 4.0". Programación FrontEnd de páginas web con HTML, CSS y JavaScript. Utilización de Git y GitHub. Conceptos fundamentales de una página web: servidores, dominios, organización de proyectos y sus etapas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +300,22 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,10 +449,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -377,17 +467,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -409,6 +520,205 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -472,7 +782,9 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -487,207 +799,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -696,7 +807,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -757,37 +870,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A13:K14" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A13:K14" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="email" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A16:L17" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <autoFilter ref="A16:L17" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="email" dataDxfId="3" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{50237959-641E-446E-B473-2F440CA62A59}" name="Linkedin" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A1:F11" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F11" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A3:F15" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A3:F15" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="4">
-      <calculatedColumnFormula>+B1+1</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="20">
+      <calculatedColumnFormula>+B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Periodo" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripcion" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Periodo" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripcion" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1056,9 +1170,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1066,186 +1180,208 @@
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="11.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="3" max="11" width="11.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>42176358</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B9" s="2">
         <v>36486</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="K16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D17" s="9">
         <v>42176358</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E17" s="9">
         <v>23</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G17" s="11">
         <v>36486</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="J17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
+      <c r="K17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I17" r:id="rId1" xr:uid="{15564F9A-7C32-4FB8-A879-CFBD9D880B8A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D90C00-5FCB-4F90-B5F9-62EA9D964F59}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,213 +1393,323 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1">
-        <f>+B2+1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>31</v>
+      <c r="F3" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1">
-        <f>+B4+1</f>
+        <f>IF(A4=A5,B4+1,1)</f>
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
+        <f t="shared" ref="B6:B15" si="0">IF(A5=A6,B5+1,1)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1">
-        <f>+B6+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C7" s="1">
-        <v>2018</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
-        <f>+B8+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C9" s="1">
-        <v>2022</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>35</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ref="B10:B11" si="0">+B9+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>2022</v>
-      </c>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>49</v>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B3DE1F-CE48-4AA1-AE35-8404F644B4EE}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("[",_xlfn.TEXTJOIN(",",TRUE,A2:A8),"]")</f>
+        <v>[Responsable,Proactivo,Trabajo en equipo,Organizado,Autodidacta,Capacidad de análisis,Resolución de problemas]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modificación de la información general
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiubaar-my.sharepoint.com/personal/jquijano_fi_uba_ar/Documents/Curso Front End -Ticmas Academy/Proyecto CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15712030-EB17-41A1-A4EF-8D2FC204D5F6}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DC044C-48BE-433F-8CC5-BC6713CC2B20}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info_personal" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
   <si>
     <t>Nombre</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Soltero</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Domicilio</t>
   </si>
   <si>
@@ -160,13 +157,7 @@
     <t>Capacitacion</t>
   </si>
   <si>
-    <t>Manejo de AutoCAD Mechanical (UBA)</t>
-  </si>
-  <si>
     <t>Curso Data Science and Machine Learning in Python</t>
-  </si>
-  <si>
-    <t>Curso Automación y Control: Módulo PLC (UTN)</t>
   </si>
   <si>
     <t>Excelente manejo de Paquete de Office</t>
@@ -282,6 +273,27 @@
   </si>
   <si>
     <t>Programa "Argentina Programa 4.0". Programación FrontEnd de páginas web con HTML, CSS y JavaScript. Utilización de Git y GitHub. Conceptos fundamentales de una página web: servidores, dominios, organización de proyectos y sus etapas.</t>
+  </si>
+  <si>
+    <t>Curso Automación y Control: Módulo PLC</t>
+  </si>
+  <si>
+    <t>UTN FRBA</t>
+  </si>
+  <si>
+    <t>FIUBA</t>
+  </si>
+  <si>
+    <t>Manejo de AutoCAD Mechanical</t>
+  </si>
+  <si>
+    <t>Fachhochschule Dortmund</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
+    <t>Array</t>
   </si>
 </sst>
 </file>
@@ -467,10 +479,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -486,6 +498,152 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -664,152 +822,6 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -870,38 +882,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A16:L17" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A16:L17" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A16:L17" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="email" dataDxfId="3" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{50237959-641E-446E-B473-2F440CA62A59}" name="Linkedin" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="Email" dataDxfId="13" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{50237959-641E-446E-B473-2F440CA62A59}" name="Linkedin" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A3:F15" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}" name="Experiencia" displayName="Experiencia" ref="A3:F15" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A3:F15" xr:uid="{67BE5B99-F3F7-4312-8C48-F36D3CBD6ECB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{1D7F1880-C9A3-48AE-92EE-5FC78EFFAE69}" name="Tipo" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{99DBE325-DE10-43C7-AC21-123995DB34A8}" name="N°" dataDxfId="4">
       <calculatedColumnFormula>+B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Periodo" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripcion" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{CAE27C65-F8E4-4BF6-B8B8-9AD50F523532}" name="Periodo" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{094E8D3C-7861-41B5-897C-E054FACCD1F5}" name="Lugar" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8D08C2B5-92C8-40AF-A90F-3440CD68A89B}" name="Titulo" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{8AC9A318-3673-45B1-BAA4-1594B9D9CA20}" name="Descripcion" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1173,7 +1185,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,8 +1197,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>75</v>
+      <c r="A1" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1199,7 +1211,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1247,34 +1259,34 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1290,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
@@ -1308,16 +1320,16 @@
         <v>11</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>6</v>
@@ -1346,19 +1358,19 @@
         <v>36486</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1380,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D90C00-5FCB-4F90-B5F9-62EA9D964F59}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,74 +1405,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>76</v>
+      <c r="A1" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <f>IF(A4=A5,B4+1,1)</f>
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B15" si="0">IF(A5=A6,B5+1,1)</f>
@@ -1469,15 +1481,15 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
@@ -1486,10 +1498,10 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1501,16 +1513,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1522,16 +1534,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>70</v>
+      <c r="F9" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1543,97 +1555,103 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
@@ -1642,10 +1660,10 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1659,54 +1677,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B3DE1F-CE48-4AA1-AE35-8404F644B4EE}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT("'",A2,"'")</f>
+        <v>'Responsable'</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT("[",_xlfn.TEXTJOIN(",",TRUE,B2:B8),"]")</f>
+        <v>['Responsable','Proactivo','Trabajo en equipo','Organizado','Autodidacta','Capacidad de análisis','Resolución de problemas']</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B8" si="0">_xlfn.CONCAT("'",A3,"'")</f>
+        <v>'Proactivo'</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A2:A8)</f>
+        <v>Responsable,Proactivo,Trabajo en equipo,Organizado,Autodidacta,Capacidad de análisis,Resolución de problemas</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Trabajo en equipo'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>'Organizado'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="str">
-        <f>_xlfn.CONCAT("[",_xlfn.TEXTJOIN(",",TRUE,A2:A8),"]")</f>
-        <v>[Responsable,Proactivo,Trabajo en equipo,Organizado,Autodidacta,Capacidad de análisis,Resolución de problemas]</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>'Autodidacta'</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Capacidad de análisis'</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>61</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>'Resolución de problemas'</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modificó el excel, quitando la información que no se usa. Se modificó también el archivo de texto por el mismo motivo.
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiubaar-my.sharepoint.com/personal/jquijano_fi_uba_ar/Documents/Curso Front End -Ticmas Academy/Proyecto CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DC044C-48BE-433F-8CC5-BC6713CC2B20}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0919F11-B3D0-474A-8DBC-541FF830A4BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="info_personal" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiencia" sheetId="2" r:id="rId2"/>
     <sheet name="Capacidades" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="infoPersonal">Datos_personales[#All]</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>Nombre</t>
   </si>
@@ -56,33 +81,6 @@
   </si>
   <si>
     <t>N°</t>
-  </si>
-  <si>
-    <t>Objetivo</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Documento</t>
-  </si>
-  <si>
-    <t>Edad</t>
-  </si>
-  <si>
-    <t>Estado_civil</t>
-  </si>
-  <si>
-    <t>Fecha_Nacimiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresar al mercado laboral con el fin de aprender y adquirir experiencia relacionada a la ingeniería mecánica. </t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Soltero</t>
   </si>
   <si>
     <t>Domicilio</t>
@@ -173,9 +171,6 @@
 Matplotlib y Scikit.learn.</t>
   </si>
   <si>
-    <t>Ingresar al mercado laboral con el fin de aprender y adquirir experiencia relacionada a la ingeniería mecánica.</t>
-  </si>
-  <si>
     <t>Periodo</t>
   </si>
   <si>
@@ -288,9 +283,6 @@
   </si>
   <si>
     <t>Fachhochschule Dortmund</t>
-  </si>
-  <si>
-    <t>Formato</t>
   </si>
   <si>
     <t>Array</t>
@@ -465,10 +457,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -477,7 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -488,7 +478,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="20">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -640,20 +630,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -663,87 +639,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
@@ -882,21 +777,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A16:L17" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="A16:L17" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A9B73725-3349-40DA-965D-C5DD6B353EC4}" name="Nacionalidad" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{D3F74730-CF31-480C-AD5F-339F450A8585}" name="Documento" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{7B88F801-5727-44F3-90CF-7A947DA98E5D}" name="Edad" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{8D7F5F4E-4D2F-48D2-AD11-5641881640BE}" name="Estado_civil" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{42737A22-D0E9-45BE-A81E-5CE1A1130E9F}" name="Fecha_Nacimiento" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="Email" dataDxfId="13" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{50237959-641E-446E-B473-2F440CA62A59}" name="Linkedin" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{223D86C4-9499-45F0-A8D1-34034ECB674B}" name="Objetivo" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}" name="Datos_personales" displayName="Datos_personales" ref="A3:F4" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A3:F4" xr:uid="{31FE2CF7-2CF4-456B-A0B2-9CB6A4BD0E2F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{318A5C80-5206-43E7-B06D-132F2C8FA583}" name="Nombre" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6068027F-12A9-41A4-8709-51FF58447C7D}" name="Profesion" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{420E7269-BE6A-441E-B97C-52ADB67545C2}" name="Domicilio" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{088F8DAE-2575-445D-BDDB-93730E39798C}" name="Email" dataDxfId="12" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="10" xr3:uid="{75227B53-5B21-4691-951A-64D75E4ECB17}" name="Celular" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{50237959-641E-446E-B473-2F440CA62A59}" name="Linkedin" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1182,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,189 +1085,106 @@
     <col min="12" max="12" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
-        <v>42176358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2">
-        <v>36486</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="9">
-        <v>42176358</v>
-      </c>
-      <c r="E17" s="9">
-        <v>23</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="11">
-        <v>36486</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="str" cm="1">
+        <f t="array" ref="A6:B11">TRANSPOSE(infoPersonal)</f>
+        <v>Nombre</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <v>Juan Pablo Quijano Cuman</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="str">
+        <v>Profesion</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <v>Estudiante de Ingeniería mecánica</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="str">
+        <v>Domicilio</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <v>Alberti  134,  Piso  7° “B”– CABA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <v>juanpquijano@outlook.com</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="str">
+        <v>Celular</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v>11-6160-3797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="str">
+        <v>Linkedin</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v>/juan-pablo-quijano-cuman</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I17" r:id="rId1" xr:uid="{15564F9A-7C32-4FB8-A879-CFBD9D880B8A}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{15564F9A-7C32-4FB8-A879-CFBD9D880B8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1393,7 +1199,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A4" sqref="A4:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1405,74 +1211,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>73</v>
+      <c r="A1" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>46</v>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
+      <c r="A4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
+      <c r="A5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <f>IF(A4=A5,B4+1,1)</f>
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
+      <c r="A6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B15" si="0">IF(A5=A6,B5+1,1)</f>
@@ -1481,15 +1287,15 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
+      <c r="A7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
@@ -1498,14 +1304,14 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1">
@@ -1513,20 +1319,20 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>71</v>
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
@@ -1534,20 +1340,20 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>67</v>
+        <v>25</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1">
@@ -1555,42 +1361,42 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
+      <c r="A11" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>38</v>
+      <c r="A12" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
@@ -1598,72 +1404,72 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>38</v>
+      <c r="A13" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>82</v>
+        <v>53</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
+      <c r="A14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>42</v>
+        <v>68</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>38</v>
+      <c r="A15" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>41</v>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1677,98 +1483,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B3DE1F-CE48-4AA1-AE35-8404F644B4EE}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="str">
-        <f>_xlfn.CONCAT("'",A2,"'")</f>
-        <v>'Responsable'</v>
-      </c>
-      <c r="D2" t="str">
-        <f>_xlfn.CONCAT("[",_xlfn.TEXTJOIN(",",TRUE,B2:B8),"]")</f>
-        <v>['Responsable','Proactivo','Trabajo en equipo','Organizado','Autodidacta','Capacidad de análisis','Resolución de problemas']</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B8" si="0">_xlfn.CONCAT("'",A3,"'")</f>
-        <v>'Proactivo'</v>
-      </c>
-      <c r="D3" t="str">
+        <v>43</v>
+      </c>
+      <c r="C3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,A2:A8)</f>
         <v>Responsable,Proactivo,Trabajo en equipo,Organizado,Autodidacta,Capacidad de análisis,Resolución de problemas</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>'Trabajo en equipo'</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>'Organizado'</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>'Autodidacta'</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>'Capacidad de análisis'</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>'Resolución de problemas'</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>